<commit_message>
Making various adjustments to lab data.
</commit_message>
<xml_diff>
--- a/38_mr_white/mr_white_data.xlsx
+++ b/38_mr_white/mr_white_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="104">
   <si>
     <t>Variable</t>
   </si>
@@ -351,6 +351,63 @@
   </si>
   <si>
     <t>148/100</t>
+  </si>
+  <si>
+    <t>Chart, Initial</t>
+  </si>
+  <si>
+    <t>Blood Test, Initial</t>
+  </si>
+  <si>
+    <t>Electrolytes, Initial</t>
+  </si>
+  <si>
+    <t>Dietary Intake, Initial</t>
+  </si>
+  <si>
+    <t>Sodium, initial</t>
+  </si>
+  <si>
+    <t>Potassium data, initial</t>
+  </si>
+  <si>
+    <t>Hormone values, initial</t>
+  </si>
+  <si>
+    <t>Sodium data, intitial</t>
+  </si>
+  <si>
+    <t>Hormonal and ion effects, initial</t>
+  </si>
+  <si>
+    <t>Glomerulal filtration rate, initial</t>
+  </si>
+  <si>
+    <t>Proximal Tubule, initial</t>
+  </si>
+  <si>
+    <t>Additional K+ and Cl- dietary treatment</t>
+  </si>
+  <si>
+    <t>Addition of AngII blockers to above treatment</t>
+  </si>
+  <si>
+    <t>Normal subject response to AngII blocker</t>
+  </si>
+  <si>
+    <t>Removing AngII blocker</t>
+  </si>
+  <si>
+    <t>Reducing salt intake</t>
+  </si>
+  <si>
+    <t>Distal tubule sodium data, after treatment</t>
+  </si>
+  <si>
+    <t>Various effects, post-treatment</t>
+  </si>
+  <si>
+    <t>Data for tumor removal in postscript</t>
   </si>
 </sst>
 </file>
@@ -775,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -786,9 +843,10 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -815,8 +873,11 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -830,7 +891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30.75" thickBot="1">
+    <row r="4" spans="1:5" ht="30.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -844,7 +905,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30.75" thickBot="1">
+    <row r="5" spans="1:5" ht="30.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -858,8 +919,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -886,8 +947,11 @@
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -901,7 +965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -915,7 +979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -929,8 +993,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="13" spans="1:4" ht="16.5" thickBot="1">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="13" spans="1:5" ht="16.5" thickBot="1">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +1008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -957,8 +1021,11 @@
       <c r="D14" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -972,7 +1039,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -986,7 +1053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -1000,7 +1067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
@@ -1014,7 +1081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30.75" thickBot="1">
+    <row r="19" spans="1:5" ht="30.75" thickBot="1">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -1028,7 +1095,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
@@ -1042,18 +1109,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75">
+    <row r="22" spans="1:5" ht="15.75">
       <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75">
+    <row r="23" spans="1:5" ht="15.75">
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1">
+    <row r="24" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="25" spans="1:5" ht="16.5" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30.75" thickBot="1">
+    <row r="26" spans="1:5" ht="30.75" thickBot="1">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -1080,8 +1147,11 @@
       <c r="D26" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30.75" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -1095,7 +1165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30.75" thickBot="1">
+    <row r="28" spans="1:5" ht="30.75" thickBot="1">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -1109,7 +1179,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30.75" thickBot="1">
+    <row r="29" spans="1:5" ht="30.75" thickBot="1">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -1123,8 +1193,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="31" spans="1:4" ht="16.5" thickBot="1">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="31" spans="1:5" ht="16.5" thickBot="1">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -1138,7 +1208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30.75" thickBot="1">
+    <row r="32" spans="1:5" ht="30.75" thickBot="1">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -1151,9 +1221,12 @@
       <c r="D32" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="34" spans="1:4" ht="16.5" thickBot="1">
+      <c r="E32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="34" spans="1:5" ht="16.5" thickBot="1">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1">
+    <row r="35" spans="1:5" ht="15.75" thickBot="1">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
@@ -1180,8 +1253,11 @@
       <c r="D35" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
@@ -1195,7 +1271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1">
+    <row r="37" spans="1:5" ht="15.75" thickBot="1">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
@@ -1209,7 +1285,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1">
+    <row r="38" spans="1:5" ht="15.75" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>44</v>
       </c>
@@ -1223,8 +1299,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="40" spans="1:4" ht="16.5" thickBot="1">
+    <row r="39" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="40" spans="1:5" ht="16.5" thickBot="1">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1">
+    <row r="41" spans="1:5" ht="15.75" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>45</v>
       </c>
@@ -1251,8 +1327,11 @@
       <c r="D41" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1">
       <c r="A42" s="3" t="s">
         <v>47</v>
       </c>
@@ -1266,7 +1345,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1">
+    <row r="43" spans="1:5" ht="15.75" thickBot="1">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
@@ -1280,7 +1359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1">
+    <row r="44" spans="1:5" ht="15.75" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -1294,7 +1373,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1">
+    <row r="45" spans="1:5" ht="15.75" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
@@ -1308,8 +1387,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="47" spans="1:4" ht="16.5" thickBot="1">
+    <row r="46" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="47" spans="1:5" ht="16.5" thickBot="1">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30.75" thickBot="1">
+    <row r="48" spans="1:5" ht="30.75" thickBot="1">
       <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
@@ -1336,8 +1415,11 @@
       <c r="D48" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30.75" thickBot="1">
       <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
@@ -1351,7 +1433,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30.75" thickBot="1">
+    <row r="50" spans="1:5" ht="30.75" thickBot="1">
       <c r="A50" s="3" t="s">
         <v>55</v>
       </c>
@@ -1365,7 +1447,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30.75" thickBot="1">
+    <row r="51" spans="1:5" ht="30.75" thickBot="1">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
@@ -1379,8 +1461,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="53" spans="1:4" ht="16.5" thickBot="1">
+    <row r="52" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="53" spans="1:5" ht="16.5" thickBot="1">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -1394,7 +1476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30.75" thickBot="1">
+    <row r="54" spans="1:5" ht="30.75" thickBot="1">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -1408,7 +1490,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30.75" thickBot="1">
+    <row r="55" spans="1:5" ht="30.75" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>58</v>
       </c>
@@ -1421,8 +1503,11 @@
       <c r="D55" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30.75" thickBot="1">
       <c r="A56" s="3" t="s">
         <v>60</v>
       </c>
@@ -1436,7 +1521,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30.75" thickBot="1">
+    <row r="57" spans="1:5" ht="30.75" thickBot="1">
       <c r="A57" s="3" t="s">
         <v>61</v>
       </c>
@@ -1450,8 +1535,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="59" spans="1:4" ht="16.5" thickBot="1">
+    <row r="58" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="59" spans="1:5" ht="16.5" thickBot="1">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -1465,7 +1550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1">
+    <row r="60" spans="1:5" ht="15.75" thickBot="1">
       <c r="A60" s="3" t="s">
         <v>62</v>
       </c>
@@ -1478,9 +1563,12 @@
       <c r="D60" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="62" spans="1:4" ht="16.5" thickBot="1">
+      <c r="E60" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="62" spans="1:5" ht="16.5" thickBot="1">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -1494,7 +1582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30.75" thickBot="1">
+    <row r="63" spans="1:5" ht="30.75" thickBot="1">
       <c r="A63" s="3" t="s">
         <v>52</v>
       </c>
@@ -1508,7 +1596,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="30.75" thickBot="1">
+    <row r="64" spans="1:5" ht="30.75" thickBot="1">
       <c r="A64" s="3" t="s">
         <v>54</v>
       </c>
@@ -1521,8 +1609,11 @@
       <c r="D64" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E64" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30.75" thickBot="1">
       <c r="A65" s="3" t="s">
         <v>55</v>
       </c>
@@ -1536,7 +1627,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="30.75" thickBot="1">
+    <row r="66" spans="1:5" ht="30.75" thickBot="1">
       <c r="A66" s="3" t="s">
         <v>64</v>
       </c>
@@ -1550,8 +1641,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="68" spans="1:4" ht="16.5" thickBot="1">
+    <row r="67" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="68" spans="1:5" ht="16.5" thickBot="1">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -1565,7 +1656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1">
+    <row r="69" spans="1:5" ht="15.75" thickBot="1">
       <c r="A69" s="3" t="s">
         <v>4</v>
       </c>
@@ -1578,8 +1669,11 @@
       <c r="D69" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E69" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" thickBot="1">
       <c r="A70" s="3" t="s">
         <v>68</v>
       </c>
@@ -1593,8 +1687,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="72" spans="1:4" ht="16.5" thickBot="1">
+    <row r="71" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="72" spans="1:5" ht="16.5" thickBot="1">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -1608,7 +1702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.75" thickBot="1">
+    <row r="73" spans="1:5" ht="15.75" thickBot="1">
       <c r="A73" s="3" t="s">
         <v>4</v>
       </c>
@@ -1621,8 +1715,11 @@
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E73" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" thickBot="1">
       <c r="A74" s="3" t="s">
         <v>68</v>
       </c>
@@ -1636,8 +1733,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="76" spans="1:4" ht="16.5" thickBot="1">
+    <row r="75" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="76" spans="1:5" ht="16.5" thickBot="1">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" thickBot="1">
+    <row r="77" spans="1:5" ht="15.75" thickBot="1">
       <c r="A77" s="3" t="s">
         <v>4</v>
       </c>
@@ -1664,8 +1761,11 @@
       <c r="D77" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E77" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" thickBot="1">
       <c r="A78" s="3" t="s">
         <v>68</v>
       </c>
@@ -1679,8 +1779,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="80" spans="1:4" ht="16.5" thickBot="1">
+    <row r="79" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="80" spans="1:5" ht="16.5" thickBot="1">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +1794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.75" thickBot="1">
+    <row r="81" spans="1:5" ht="15.75" thickBot="1">
       <c r="A81" s="3" t="s">
         <v>4</v>
       </c>
@@ -1707,8 +1807,11 @@
       <c r="D81" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickBot="1">
       <c r="A82" s="3" t="s">
         <v>68</v>
       </c>
@@ -1722,8 +1825,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="84" spans="1:4" ht="16.5" thickBot="1">
+    <row r="83" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="84" spans="1:5" ht="16.5" thickBot="1">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -1737,7 +1840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.75" thickBot="1">
+    <row r="85" spans="1:5" ht="15.75" thickBot="1">
       <c r="A85" s="3" t="s">
         <v>4</v>
       </c>
@@ -1750,8 +1853,11 @@
       <c r="D85" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E85" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" thickBot="1">
       <c r="A86" s="3" t="s">
         <v>68</v>
       </c>
@@ -1765,8 +1871,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="88" spans="1:4" ht="16.5" thickBot="1">
+    <row r="87" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="88" spans="1:5" ht="16.5" thickBot="1">
       <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
@@ -1780,7 +1886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="30.75" thickBot="1">
+    <row r="89" spans="1:5" ht="30.75" thickBot="1">
       <c r="A89" s="3" t="s">
         <v>52</v>
       </c>
@@ -1793,8 +1899,11 @@
       <c r="D89" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E89" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="30.75" thickBot="1">
       <c r="A90" s="3" t="s">
         <v>54</v>
       </c>
@@ -1808,7 +1917,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="30.75" thickBot="1">
+    <row r="91" spans="1:5" ht="30.75" thickBot="1">
       <c r="A91" s="3" t="s">
         <v>55</v>
       </c>
@@ -1822,7 +1931,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="30.75" thickBot="1">
+    <row r="92" spans="1:5" ht="30.75" thickBot="1">
       <c r="A92" s="3" t="s">
         <v>64</v>
       </c>
@@ -1836,8 +1945,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="94" spans="1:4" ht="16.5" thickBot="1">
+    <row r="93" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="94" spans="1:5" ht="16.5" thickBot="1">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
@@ -1851,7 +1960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="30.75" thickBot="1">
+    <row r="95" spans="1:5" ht="30.75" thickBot="1">
       <c r="A95" s="3" t="s">
         <v>57</v>
       </c>
@@ -1864,8 +1973,11 @@
       <c r="D95" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E95" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="30.75" thickBot="1">
       <c r="A96" s="3" t="s">
         <v>58</v>
       </c>
@@ -1879,7 +1991,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="30.75" thickBot="1">
+    <row r="97" spans="1:5" ht="30.75" thickBot="1">
       <c r="A97" s="3" t="s">
         <v>60</v>
       </c>
@@ -1893,7 +2005,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="30.75" thickBot="1">
+    <row r="98" spans="1:5" ht="30.75" thickBot="1">
       <c r="A98" s="3" t="s">
         <v>61</v>
       </c>
@@ -1907,12 +2019,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="30.75" thickBot="1">
+    <row r="100" spans="1:5" ht="30.75" thickBot="1">
       <c r="A100" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="32.25" thickBot="1">
+    <row r="101" spans="1:5" ht="32.25" thickBot="1">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +2038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.75" thickBot="1">
+    <row r="102" spans="1:5" ht="15.75" thickBot="1">
       <c r="A102" s="3" t="s">
         <v>4</v>
       </c>
@@ -1939,8 +2051,11 @@
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E102" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15.75" thickBot="1">
       <c r="A103" s="3" t="s">
         <v>68</v>
       </c>
@@ -1956,7 +2071,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>